<commit_message>
adding ATPase R files and jpegs
</commit_message>
<xml_diff>
--- a/ATPase data sheet.xlsx
+++ b/ATPase data sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltroo\Documents\Git\Clam-OA-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD5CE09-4C5B-4145-ADE1-315B1E593E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836C2C7A-FB48-4FB7-9C01-DFD15A0275E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9CFE1E20-EF3C-4183-819B-479C0FD4C980}"/>
+    <workbookView xWindow="1044" yWindow="1044" windowWidth="7500" windowHeight="6000" xr2:uid="{9CFE1E20-EF3C-4183-819B-479C0FD4C980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="152">
   <si>
     <t>A</t>
   </si>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B47173-9419-4988-ABFA-099541913FA8}">
   <dimension ref="A1:I140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,18 +906,18 @@
         <v>23.93</v>
       </c>
       <c r="F2">
-        <f>D2-E2</f>
+        <f t="shared" ref="F2:F33" si="0">D2-E2</f>
         <v>1.870000000000001</v>
       </c>
       <c r="G2">
         <v>19.472000000000001</v>
       </c>
       <c r="H2">
-        <f>(F2/G2)*(60/20)</f>
+        <f t="shared" ref="H2:H21" si="1">(F2/G2)*(60/20)</f>
         <v>0.28810599835661477</v>
       </c>
       <c r="I2">
-        <f>D2/G2</f>
+        <f t="shared" ref="I2:I21" si="2">D2/G2</f>
         <v>1.3249794576828267</v>
       </c>
     </row>
@@ -938,18 +938,18 @@
         <v>34.69</v>
       </c>
       <c r="F3">
-        <f>D3-E3</f>
+        <f t="shared" si="0"/>
         <v>2.4699999999999989</v>
       </c>
       <c r="G3">
         <v>18.341000000000001</v>
       </c>
       <c r="H3">
-        <f>(F3/G3)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.4040128673463822</v>
       </c>
       <c r="I3">
-        <f>D3/G3</f>
+        <f t="shared" si="2"/>
         <v>2.0260618286898202</v>
       </c>
     </row>
@@ -970,18 +970,18 @@
         <v>39.68</v>
       </c>
       <c r="F4">
-        <f>D4-E4</f>
+        <f t="shared" si="0"/>
         <v>4.8500000000000014</v>
       </c>
       <c r="G4">
         <v>20.417000000000002</v>
       </c>
       <c r="H4">
-        <f>(F4/G4)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.71264142626242855</v>
       </c>
       <c r="I4">
-        <f>D4/G4</f>
+        <f t="shared" si="2"/>
         <v>2.1810256159083115</v>
       </c>
     </row>
@@ -1002,18 +1002,18 @@
         <v>38.020000000000003</v>
       </c>
       <c r="F5">
-        <f>D5-E5</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="G5">
         <v>16.016999999999999</v>
       </c>
       <c r="H5">
-        <f>(F5/G5)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.42142723356433787</v>
       </c>
       <c r="I5">
-        <f>D5/G5</f>
+        <f t="shared" si="2"/>
         <v>2.5142036586127241</v>
       </c>
     </row>
@@ -1034,18 +1034,18 @@
         <v>30.74</v>
       </c>
       <c r="F6">
-        <f>D6-E6</f>
+        <f t="shared" si="0"/>
         <v>1.9800000000000004</v>
       </c>
       <c r="G6">
         <v>16.436</v>
       </c>
       <c r="H6">
-        <f>(F6/G6)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.36140180092479929</v>
       </c>
       <c r="I6">
-        <f>D6/G6</f>
+        <f t="shared" si="2"/>
         <v>1.9907520077877829</v>
       </c>
     </row>
@@ -1066,18 +1066,18 @@
         <v>33.6</v>
       </c>
       <c r="F7">
-        <f>D7-E7</f>
+        <f t="shared" si="0"/>
         <v>4.57</v>
       </c>
       <c r="G7">
         <v>24.873999999999999</v>
       </c>
       <c r="H7">
-        <f>(F7/G7)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.55117793680147953</v>
       </c>
       <c r="I7">
-        <f>D7/G7</f>
+        <f t="shared" si="2"/>
         <v>1.5345340516201658</v>
       </c>
     </row>
@@ -1098,18 +1098,18 @@
         <v>28.57</v>
       </c>
       <c r="F8">
-        <f>D8-E8</f>
+        <f t="shared" si="0"/>
         <v>8.7999999999999972</v>
       </c>
       <c r="G8">
         <v>23.52</v>
       </c>
       <c r="H8">
-        <f>(F8/G8)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>1.1224489795918364</v>
       </c>
       <c r="I8">
-        <f>D8/G8</f>
+        <f t="shared" si="2"/>
         <v>1.5888605442176871</v>
       </c>
     </row>
@@ -1130,18 +1130,18 @@
         <v>27.88</v>
       </c>
       <c r="F9">
-        <f>D9-E9</f>
+        <f t="shared" si="0"/>
         <v>2.0800000000000018</v>
       </c>
       <c r="G9">
         <v>18.236000000000001</v>
       </c>
       <c r="H9">
-        <f>(F9/G9)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.3421803026979604</v>
       </c>
       <c r="I9">
-        <f>D9/G9</f>
+        <f t="shared" si="2"/>
         <v>1.642904145645975</v>
       </c>
     </row>
@@ -1162,18 +1162,18 @@
         <v>33.01</v>
       </c>
       <c r="F10">
-        <f>D10-E10</f>
+        <f t="shared" si="0"/>
         <v>5.3900000000000006</v>
       </c>
       <c r="G10">
         <v>19.376999999999999</v>
       </c>
       <c r="H10">
-        <f>(F10/G10)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.83449450379315704</v>
       </c>
       <c r="I10">
-        <f>D10/G10</f>
+        <f t="shared" si="2"/>
         <v>1.981730918098777</v>
       </c>
     </row>
@@ -1194,18 +1194,18 @@
         <v>26.4</v>
       </c>
       <c r="F11">
-        <f>D11-E11</f>
+        <f t="shared" si="0"/>
         <v>5.57</v>
       </c>
       <c r="G11">
         <v>19.021999999999998</v>
       </c>
       <c r="H11">
-        <f>(F11/G11)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.87845652402481356</v>
       </c>
       <c r="I11">
-        <f>D11/G11</f>
+        <f t="shared" si="2"/>
         <v>1.6806855220271266</v>
       </c>
     </row>
@@ -1226,18 +1226,18 @@
         <v>30.88</v>
       </c>
       <c r="F12">
-        <f>D12-E12</f>
+        <f t="shared" si="0"/>
         <v>6.98</v>
       </c>
       <c r="G12">
         <v>19.907</v>
       </c>
       <c r="H12">
-        <f>(F12/G12)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>1.0518912945195158</v>
       </c>
       <c r="I12">
-        <f>D12/G12</f>
+        <f t="shared" si="2"/>
         <v>1.9018435726126488</v>
       </c>
     </row>
@@ -1258,18 +1258,18 @@
         <v>42.34</v>
       </c>
       <c r="F13">
-        <f>D13-E13</f>
+        <f t="shared" si="0"/>
         <v>9.4199999999999946</v>
       </c>
       <c r="G13">
         <v>31.93</v>
       </c>
       <c r="H13">
-        <f>(F13/G13)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.88506107109301546</v>
       </c>
       <c r="I13">
-        <f>D13/G13</f>
+        <f t="shared" si="2"/>
         <v>1.6210460382085812</v>
       </c>
     </row>
@@ -1290,18 +1290,18 @@
         <v>21.298999999999999</v>
       </c>
       <c r="F14">
-        <f>D14-E14</f>
+        <f t="shared" si="0"/>
         <v>0.97299999999999898</v>
       </c>
       <c r="G14">
         <v>10.359</v>
       </c>
       <c r="H14">
-        <f>(F14/G14)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.2817839559803067</v>
       </c>
       <c r="I14">
-        <f>D14/G14</f>
+        <f t="shared" si="2"/>
         <v>2.1500144801621777</v>
       </c>
     </row>
@@ -1322,18 +1322,18 @@
         <v>24.486000000000001</v>
       </c>
       <c r="F15">
-        <f>D15-E15</f>
+        <f t="shared" si="0"/>
         <v>5.4719999999999978</v>
       </c>
       <c r="G15">
         <v>14.429</v>
       </c>
       <c r="H15">
-        <f>(F15/G15)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>1.1377087809272988</v>
       </c>
       <c r="I15">
-        <f>D15/G15</f>
+        <f t="shared" si="2"/>
         <v>2.0762353593457616</v>
       </c>
     </row>
@@ -1354,18 +1354,18 @@
         <v>28.218</v>
       </c>
       <c r="F16">
-        <f>D16-E16</f>
+        <f t="shared" si="0"/>
         <v>3.1389999999999993</v>
       </c>
       <c r="G16">
         <v>13.465</v>
       </c>
       <c r="H16">
-        <f>(F16/G16)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.69936873375417741</v>
       </c>
       <c r="I16">
-        <f>D16/G16</f>
+        <f t="shared" si="2"/>
         <v>2.3287783141477907</v>
       </c>
     </row>
@@ -1386,18 +1386,18 @@
         <v>38.89</v>
       </c>
       <c r="F17">
-        <f>D17-E17</f>
+        <f t="shared" si="0"/>
         <v>6.4500000000000028</v>
       </c>
       <c r="G17">
         <v>21.875</v>
       </c>
       <c r="H17">
-        <f>(F17/G17)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.88457142857142901</v>
       </c>
       <c r="I17">
-        <f>D17/G17</f>
+        <f t="shared" si="2"/>
         <v>2.0726857142857145</v>
       </c>
     </row>
@@ -1418,18 +1418,18 @@
         <v>35.279000000000003</v>
       </c>
       <c r="F18">
-        <f>D18-E18</f>
+        <f t="shared" si="0"/>
         <v>5.0640000000000001</v>
       </c>
       <c r="G18">
         <v>19.760999999999999</v>
       </c>
       <c r="H18">
-        <f>(F18/G18)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.76878700470623973</v>
       </c>
       <c r="I18">
-        <f>D18/G18</f>
+        <f t="shared" si="2"/>
         <v>2.0415464804412733</v>
       </c>
     </row>
@@ -1450,18 +1450,18 @@
         <v>28.696999999999999</v>
       </c>
       <c r="F19">
-        <f>D19-E19</f>
+        <f t="shared" si="0"/>
         <v>3.1280000000000001</v>
       </c>
       <c r="G19">
         <v>17.887</v>
       </c>
       <c r="H19">
-        <f>(F19/G19)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.52462682395035498</v>
       </c>
       <c r="I19">
-        <f>D19/G19</f>
+        <f t="shared" si="2"/>
         <v>1.7792251355733213</v>
       </c>
     </row>
@@ -1482,18 +1482,18 @@
         <v>20.727</v>
       </c>
       <c r="F20">
-        <f>D20-E20</f>
+        <f t="shared" si="0"/>
         <v>2.5279999999999987</v>
       </c>
       <c r="G20">
         <v>14.885999999999999</v>
       </c>
       <c r="H20">
-        <f>(F20/G20)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.50947198710197483</v>
       </c>
       <c r="I20">
-        <f>D20/G20</f>
+        <f t="shared" si="2"/>
         <v>1.5622060996909848</v>
       </c>
     </row>
@@ -1514,18 +1514,18 @@
         <v>28.32</v>
       </c>
       <c r="F21">
-        <f>D21-E21</f>
+        <f t="shared" si="0"/>
         <v>4.3399999999999963</v>
       </c>
       <c r="G21">
         <v>15.989000000000001</v>
       </c>
       <c r="H21">
-        <f>(F21/G21)*(60/20)</f>
+        <f t="shared" si="1"/>
         <v>0.81430983801363366</v>
       </c>
       <c r="I21">
-        <f>D21/G21</f>
+        <f t="shared" si="2"/>
         <v>2.0426543248483329</v>
       </c>
     </row>
@@ -1546,8 +1546,19 @@
         <v>22.141999999999999</v>
       </c>
       <c r="F22">
-        <f>D22-E22</f>
+        <f t="shared" si="0"/>
         <v>18.943999999999999</v>
+      </c>
+      <c r="G22">
+        <v>24.75</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:H85" si="3">(F22/G22)*(60/20)</f>
+        <v>2.2962424242424238</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I85" si="4">D22/G22</f>
+        <v>1.660040404040404</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1567,8 +1578,19 @@
         <v>25.224</v>
       </c>
       <c r="F23">
-        <f>D23-E23</f>
+        <f t="shared" si="0"/>
         <v>23.699000000000002</v>
+      </c>
+      <c r="G23">
+        <v>33.926000000000002</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>2.0956493544773922</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>1.4420503448682427</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1588,8 +1610,19 @@
         <v>27.731999999999999</v>
       </c>
       <c r="F24">
-        <f>D24-E24</f>
+        <f t="shared" si="0"/>
         <v>31.636000000000003</v>
+      </c>
+      <c r="G24">
+        <v>31.93</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>2.9723770748512375</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1.8593172564985907</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1609,8 +1642,19 @@
         <v>19.635000000000002</v>
       </c>
       <c r="F25">
-        <f>D25-E25</f>
+        <f t="shared" si="0"/>
         <v>30.292999999999996</v>
+      </c>
+      <c r="G25">
+        <v>33.15</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>2.7414479638009048</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>1.5061236802413274</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1630,8 +1674,19 @@
         <v>25.279</v>
       </c>
       <c r="F26">
-        <f>D26-E26</f>
+        <f t="shared" si="0"/>
         <v>30.191999999999997</v>
+      </c>
+      <c r="G26">
+        <v>34.49</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>2.626152507973325</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>1.608321252536967</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1651,8 +1706,19 @@
         <v>26.425000000000001</v>
       </c>
       <c r="F27">
-        <f>D27-E27</f>
+        <f t="shared" si="0"/>
         <v>59.868000000000009</v>
+      </c>
+      <c r="G27">
+        <v>45.804000000000002</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>3.9211422583180511</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>1.8839620993799668</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1672,8 +1738,19 @@
         <v>24.343</v>
       </c>
       <c r="F28">
-        <f>D28-E28</f>
+        <f t="shared" si="0"/>
         <v>22.488000000000003</v>
+      </c>
+      <c r="G28">
+        <v>24.923999999999999</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>2.7067886374578727</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>1.8789520141229339</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1693,8 +1770,19 @@
         <v>21.675000000000001</v>
       </c>
       <c r="F29">
-        <f>D29-E29</f>
+        <f t="shared" si="0"/>
         <v>27.352999999999998</v>
+      </c>
+      <c r="G29">
+        <v>37.896000000000001</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>2.1653736542115261</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>1.2937513194004644</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1714,8 +1802,19 @@
         <v>25.268999999999998</v>
       </c>
       <c r="F30">
-        <f>D30-E30</f>
+        <f t="shared" si="0"/>
         <v>24.023000000000003</v>
+      </c>
+      <c r="G30">
+        <v>33.770000000000003</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>2.1341131181522064</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="4"/>
+        <v>1.4596387326029019</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1735,8 +1834,19 @@
         <v>14.33</v>
       </c>
       <c r="F31">
-        <f>D31-E31</f>
+        <f t="shared" si="0"/>
         <v>11.578000000000001</v>
+      </c>
+      <c r="G31">
+        <v>15.53</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>2.2365743721828721</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>1.6682549903412751</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1756,11 +1866,22 @@
         <v>21.577999999999999</v>
       </c>
       <c r="F32">
-        <f>D32-E32</f>
+        <f t="shared" si="0"/>
         <v>28.510999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>32.537999999999997</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>2.6287110455467455</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
+        <v>1.5394000860532302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1777,11 +1898,22 @@
         <v>20.317</v>
       </c>
       <c r="F33">
-        <f>D33-E33</f>
+        <f t="shared" si="0"/>
         <v>15.962000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>23.198</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>2.0642296749719806</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="4"/>
+        <v>1.5638848176566946</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -1798,11 +1930,22 @@
         <v>20.701000000000001</v>
       </c>
       <c r="F34">
-        <f>D34-E34</f>
+        <f t="shared" ref="F34:F65" si="5">D34-E34</f>
         <v>12.125</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>19.956</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>1.8227600721587491</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
+        <v>1.6449188214070958</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1819,11 +1962,22 @@
         <v>28.053000000000001</v>
       </c>
       <c r="F35">
-        <f>D35-E35</f>
+        <f t="shared" si="5"/>
         <v>13.513999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>34.822000000000003</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>1.1642639710527825</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>1.1936993854459823</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1840,11 +1994,22 @@
         <v>14.125</v>
       </c>
       <c r="F36">
-        <f>D36-E36</f>
+        <f t="shared" si="5"/>
         <v>7.8539999999999992</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>13.936</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>1.6907290470723304</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>1.577138346727899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1861,11 +2026,22 @@
         <v>22.751000000000001</v>
       </c>
       <c r="F37">
-        <f>D37-E37</f>
+        <f t="shared" si="5"/>
         <v>19.203999999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>28.98</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>1.9879917184265006</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
+        <v>1.4477225672877847</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1882,11 +2058,22 @@
         <v>21.751999999999999</v>
       </c>
       <c r="F38">
-        <f>D38-E38</f>
+        <f t="shared" si="5"/>
         <v>12.854000000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>28.963999999999999</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>1.3313768816461817</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>1.194793536804309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1903,11 +2090,22 @@
         <v>12.742000000000001</v>
       </c>
       <c r="F39">
-        <f>D39-E39</f>
+        <f t="shared" si="5"/>
         <v>8.7330000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>15.438000000000001</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>1.6970462495141856</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>1.3910480632206246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1924,11 +2122,22 @@
         <v>21.015000000000001</v>
       </c>
       <c r="F40">
-        <f>D40-E40</f>
+        <f t="shared" si="5"/>
         <v>18.429000000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>29.43</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>1.8785932721712542</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>1.3402650356778798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1945,11 +2154,22 @@
         <v>30.346</v>
       </c>
       <c r="F41">
-        <f>D41-E41</f>
+        <f t="shared" si="5"/>
         <v>24.995999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>41.558</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="3"/>
+        <v>1.8044179219404204</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>1.3316810241108812</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1966,11 +2186,22 @@
         <v>26.14</v>
       </c>
       <c r="F42">
-        <f>D42-E42</f>
+        <f t="shared" si="5"/>
         <v>18.070999999999998</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>23.416</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="3"/>
+        <v>2.3152118209771091</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="4"/>
+        <v>1.8880679877007174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1987,11 +2218,22 @@
         <v>14.378</v>
       </c>
       <c r="F43">
-        <f>D43-E43</f>
+        <f t="shared" si="5"/>
         <v>6.4939999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>12.981999999999999</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="3"/>
+        <v>1.5006932676012941</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="4"/>
+        <v>1.607764597134494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
@@ -2008,11 +2250,22 @@
         <v>29.661000000000001</v>
       </c>
       <c r="F44">
-        <f>D44-E44</f>
+        <f t="shared" si="5"/>
         <v>18.213999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="3"/>
+        <v>1.6335426008968608</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="4"/>
+        <v>1.4312406576980568</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -2029,11 +2282,22 @@
         <v>32.343000000000004</v>
       </c>
       <c r="F45">
-        <f>D45-E45</f>
+        <f t="shared" si="5"/>
         <v>25.114999999999995</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>37.625999999999998</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="3"/>
+        <v>2.002471695104449</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
+        <v>1.5270823366820816</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>34</v>
       </c>
@@ -2050,11 +2314,22 @@
         <v>28.215</v>
       </c>
       <c r="F46">
-        <f>D46-E46</f>
+        <f t="shared" si="5"/>
         <v>32.703000000000003</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>35.341999999999999</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="3"/>
+        <v>2.7759889083809632</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>1.7236715522607662</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -2071,11 +2346,22 @@
         <v>20.452000000000002</v>
       </c>
       <c r="F47">
-        <f>D47-E47</f>
+        <f t="shared" si="5"/>
         <v>14.108999999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>23.498000000000001</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="3"/>
+        <v>1.8013022384883817</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="4"/>
+        <v>1.4708060260447697</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -2092,11 +2378,22 @@
         <v>25.574000000000002</v>
       </c>
       <c r="F48">
-        <f>D48-E48</f>
+        <f t="shared" si="5"/>
         <v>37.025999999999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>31.844000000000001</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="3"/>
+        <v>3.4881924381359122</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="4"/>
+        <v>1.9658334380103002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -2113,11 +2410,22 @@
         <v>23.297000000000001</v>
       </c>
       <c r="F49">
-        <f>D49-E49</f>
+        <f t="shared" si="5"/>
         <v>21.040000000000003</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>26.448</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="3"/>
+        <v>2.3865698729582578</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="4"/>
+        <v>1.6763838475499093</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -2134,11 +2442,22 @@
         <v>26.74</v>
       </c>
       <c r="F50">
-        <f>D50-E50</f>
+        <f t="shared" si="5"/>
         <v>26.165000000000003</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>26.204000000000001</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="3"/>
+        <v>2.9955350328194172</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="4"/>
+        <v>2.0189665699893147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -2155,11 +2474,22 @@
         <v>24.013999999999999</v>
       </c>
       <c r="F51">
-        <f>D51-E51</f>
+        <f t="shared" si="5"/>
         <v>13.727</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>23.79</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="3"/>
+        <v>1.7310214375788147</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="4"/>
+        <v>1.5864228667507356</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>40</v>
       </c>
@@ -2176,11 +2506,22 @@
         <v>25.766999999999999</v>
       </c>
       <c r="F52">
-        <f>D52-E52</f>
+        <f t="shared" si="5"/>
         <v>20.279</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>32.021999999999998</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="3"/>
+        <v>1.8998501030541504</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="4"/>
+        <v>1.4379489101242895</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -2197,11 +2538,22 @@
         <v>20.824999999999999</v>
       </c>
       <c r="F53">
-        <f>D53-E53</f>
+        <f t="shared" si="5"/>
         <v>18.318999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>22.878</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="3"/>
+        <v>2.4021767637031206</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="4"/>
+        <v>1.7109887227904537</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>42</v>
       </c>
@@ -2218,11 +2570,22 @@
         <v>17.641999999999999</v>
       </c>
       <c r="F54">
-        <f>D54-E54</f>
+        <f t="shared" si="5"/>
         <v>9.9849999999999994</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>24.474</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="3"/>
+        <v>1.2239519490071094</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="4"/>
+        <v>1.1288305957342486</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -2239,11 +2602,22 @@
         <v>24.459</v>
       </c>
       <c r="F55">
-        <f>D55-E55</f>
+        <f t="shared" si="5"/>
         <v>13.891999999999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>27.31</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="3"/>
+        <v>1.5260344196265105</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="4"/>
+        <v>1.4042841450018309</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -2260,11 +2634,22 @@
         <v>18.268999999999998</v>
       </c>
       <c r="F56">
-        <f>D56-E56</f>
+        <f t="shared" si="5"/>
         <v>8.6320000000000014</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>23.562000000000001</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="3"/>
+        <v>1.099057804940158</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="4"/>
+        <v>1.141711229946524</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
@@ -2281,11 +2666,22 @@
         <v>26.238</v>
       </c>
       <c r="F57">
-        <f>D57-E57</f>
+        <f t="shared" si="5"/>
         <v>16.308999999999997</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>31.67</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="3"/>
+        <v>1.5449005367856015</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="4"/>
+        <v>1.3434480580991472</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -2302,11 +2698,22 @@
         <v>23.032</v>
       </c>
       <c r="F58">
-        <f>D58-E58</f>
+        <f t="shared" si="5"/>
         <v>29.407999999999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>33.286000000000001</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="3"/>
+        <v>2.6504836868353059</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="4"/>
+        <v>1.5754371207114102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -2323,11 +2730,22 @@
         <v>18.233000000000001</v>
       </c>
       <c r="F59">
-        <f>D59-E59</f>
+        <f t="shared" si="5"/>
         <v>12.567</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>21.036000000000001</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="3"/>
+        <v>1.7922133485453509</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="4"/>
+        <v>1.4641566837801863</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -2344,11 +2762,22 @@
         <v>21.783000000000001</v>
       </c>
       <c r="F60">
-        <f>D60-E60</f>
+        <f t="shared" si="5"/>
         <v>12.964999999999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>22.89</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="3"/>
+        <v>1.6992136304062904</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="4"/>
+        <v>1.5180428134556574</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
@@ -2365,11 +2794,22 @@
         <v>16.687000000000001</v>
       </c>
       <c r="F61">
-        <f>D61-E61</f>
+        <f t="shared" si="5"/>
         <v>31.477</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>26.571999999999999</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="3"/>
+        <v>3.5537784133674548</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="4"/>
+        <v>1.8125846755983743</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -2386,11 +2826,22 @@
         <v>24.190999999999999</v>
       </c>
       <c r="F62">
-        <f>D62-E62</f>
+        <f t="shared" si="5"/>
         <v>21.257999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>27.417999999999999</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="3"/>
+        <v>2.3259902253993729</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="4"/>
+        <v>1.6576336713108177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -2407,11 +2858,22 @@
         <v>24.771000000000001</v>
       </c>
       <c r="F63">
-        <f>D63-E63</f>
+        <f t="shared" si="5"/>
         <v>15.683</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>21.86</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="3"/>
+        <v>2.152287282708143</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="4"/>
+        <v>1.8505946935041171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -2428,11 +2890,22 @@
         <v>27.946000000000002</v>
       </c>
       <c r="F64">
-        <f>D64-E64</f>
+        <f t="shared" si="5"/>
         <v>23.084999999999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>28.228000000000002</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="3"/>
+        <v>2.4534150488876287</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="4"/>
+        <v>1.8078149355250104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -2449,11 +2922,22 @@
         <v>34.348999999999997</v>
       </c>
       <c r="F65">
-        <f>D65-E65</f>
+        <f t="shared" si="5"/>
         <v>33.663000000000004</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>40.822000000000003</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="3"/>
+        <v>2.4738866297584639</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="4"/>
+        <v>1.666062417323992</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -2470,11 +2954,22 @@
         <v>17.109000000000002</v>
       </c>
       <c r="F66">
-        <f>D66-E66</f>
+        <f t="shared" ref="F66:F97" si="6">D66-E66</f>
         <v>10.117999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>17.867999999999999</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="3"/>
+        <v>1.6987911349899261</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="4"/>
+        <v>1.5237855383926575</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -2491,11 +2986,22 @@
         <v>19.571999999999999</v>
       </c>
       <c r="F67">
-        <f>D67-E67</f>
+        <f t="shared" si="6"/>
         <v>13.695000000000004</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>22.3</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="3"/>
+        <v>1.8423766816143501</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="4"/>
+        <v>1.4917937219730943</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -2512,11 +3018,22 @@
         <v>22.509</v>
       </c>
       <c r="F68">
-        <f>D68-E68</f>
+        <f t="shared" si="6"/>
         <v>17.497</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>25.622</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>2.0486691124814613</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="4"/>
+        <v>1.5613925532745296</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
@@ -2533,11 +3050,22 @@
         <v>22.094000000000001</v>
       </c>
       <c r="F69">
-        <f>D69-E69</f>
+        <f t="shared" si="6"/>
         <v>19.112000000000002</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>23.207999999999998</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="3"/>
+        <v>2.4705274043433301</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="4"/>
+        <v>1.775508445363668</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -2554,11 +3082,22 @@
         <v>20.777999999999999</v>
       </c>
       <c r="F70">
-        <f>D70-E70</f>
+        <f t="shared" si="6"/>
         <v>14.602000000000004</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>26.48</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="3"/>
+        <v>1.6543051359516618</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="4"/>
+        <v>1.3361027190332326</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>59</v>
       </c>
@@ -2575,11 +3114,22 @@
         <v>26.994</v>
       </c>
       <c r="F71">
-        <f>D71-E71</f>
+        <f t="shared" si="6"/>
         <v>19.716000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>20.47</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="3"/>
+        <v>2.8894968246213972</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="4"/>
+        <v>2.2818759159745969</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -2596,11 +3146,22 @@
         <v>24.823</v>
       </c>
       <c r="F72">
-        <f>D72-E72</f>
+        <f t="shared" si="6"/>
         <v>13.645000000000003</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>28.66</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="3"/>
+        <v>1.4282972784368462</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="4"/>
+        <v>1.3422191207257503</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>61</v>
       </c>
@@ -2617,11 +3178,22 @@
         <v>21.870999999999999</v>
       </c>
       <c r="F73">
-        <f>D73-E73</f>
+        <f t="shared" si="6"/>
         <v>28.937999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>25.904</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="3"/>
+        <v>3.3513743051266207</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="4"/>
+        <v>1.9614345274861025</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -2638,11 +3210,22 @@
         <v>22.905000000000001</v>
       </c>
       <c r="F74">
-        <f>D74-E74</f>
+        <f t="shared" si="6"/>
         <v>26.591999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>25.74</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="3"/>
+        <v>3.0993006993006991</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="4"/>
+        <v>1.922960372960373</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
@@ -2659,11 +3242,22 @@
         <v>29.896000000000001</v>
       </c>
       <c r="F75">
-        <f>D75-E75</f>
+        <f t="shared" si="6"/>
         <v>28.646000000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>40.450000000000003</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="3"/>
+        <v>2.1245488257107539</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="4"/>
+        <v>1.4472682323856612</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>64</v>
       </c>
@@ -2680,11 +3274,22 @@
         <v>26.555</v>
       </c>
       <c r="F76">
-        <f>D76-E76</f>
+        <f t="shared" si="6"/>
         <v>42.318000000000005</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>39.594000000000001</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="3"/>
+        <v>3.2063949083194427</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="4"/>
+        <v>1.7394807294034451</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>65</v>
       </c>
@@ -2701,11 +3306,22 @@
         <v>25.167000000000002</v>
       </c>
       <c r="F77">
-        <f>D77-E77</f>
+        <f t="shared" si="6"/>
         <v>16.869999999999997</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <v>22.898</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="3"/>
+        <v>2.2102367018953615</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="4"/>
+        <v>1.8358371910210498</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -2722,11 +3338,22 @@
         <v>26.268999999999998</v>
       </c>
       <c r="F78">
-        <f>D78-E78</f>
+        <f t="shared" si="6"/>
         <v>23.189</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <v>23.782</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="3"/>
+        <v>2.9251955260280886</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="4"/>
+        <v>2.0796400639138843</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>128</v>
       </c>
@@ -2743,11 +3370,22 @@
         <v>17.585000000000001</v>
       </c>
       <c r="F79">
-        <f>D79-E79</f>
+        <f t="shared" si="6"/>
         <v>13.143999999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <v>16.986000000000001</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="3"/>
+        <v>2.3214411868597664</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="4"/>
+        <v>1.8090780642882374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>129</v>
       </c>
@@ -2764,11 +3402,22 @@
         <v>25.707000000000001</v>
       </c>
       <c r="F80">
-        <f>D80-E80</f>
+        <f t="shared" si="6"/>
         <v>26.136000000000003</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <v>24.271999999999998</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="3"/>
+        <v>3.2303889255108773</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="4"/>
+        <v>2.1359179301252476</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>130</v>
       </c>
@@ -2785,11 +3434,22 @@
         <v>25.478999999999999</v>
       </c>
       <c r="F81">
-        <f>D81-E81</f>
+        <f t="shared" si="6"/>
         <v>33.975000000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <v>30.494</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="3"/>
+        <v>3.3424608119630097</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="4"/>
+        <v>1.9496950219715354</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>131</v>
       </c>
@@ -2806,11 +3466,22 @@
         <v>17.844000000000001</v>
       </c>
       <c r="F82">
-        <f>D82-E82</f>
+        <f t="shared" si="6"/>
         <v>8.5299999999999976</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <v>20.88</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="3"/>
+        <v>1.2255747126436778</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="4"/>
+        <v>1.2631226053639846</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>132</v>
       </c>
@@ -2827,11 +3498,22 @@
         <v>15.486000000000001</v>
       </c>
       <c r="F83">
-        <f>D83-E83</f>
+        <f t="shared" si="6"/>
         <v>7.1400000000000006</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <v>20.56</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="3"/>
+        <v>1.0418287937743191</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="4"/>
+        <v>1.1004863813229573</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>133</v>
       </c>
@@ -2848,11 +3530,22 @@
         <v>24.472000000000001</v>
       </c>
       <c r="F84">
-        <f>D84-E84</f>
+        <f t="shared" si="6"/>
         <v>17.152000000000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <v>21.13</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="3"/>
+        <v>2.4352106010411738</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="4"/>
+        <v>1.9699006152389968</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>134</v>
       </c>
@@ -2869,11 +3562,22 @@
         <v>28.52</v>
       </c>
       <c r="F85">
-        <f>D85-E85</f>
+        <f t="shared" si="6"/>
         <v>12.378000000000004</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <v>26.638000000000002</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="3"/>
+        <v>1.3940235753434946</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="4"/>
+        <v>1.5353254748855019</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>135</v>
       </c>
@@ -2890,11 +3594,22 @@
         <v>23.465</v>
       </c>
       <c r="F86">
-        <f>D86-E86</f>
+        <f t="shared" si="6"/>
         <v>16.474</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <v>19.835999999999999</v>
+      </c>
+      <c r="H86">
+        <f t="shared" ref="H86:H140" si="7">(F86/G86)*(60/20)</f>
+        <v>2.4915305505142169</v>
+      </c>
+      <c r="I86">
+        <f t="shared" ref="I86:I140" si="8">D86/G86</f>
+        <v>2.0134603750756201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>66</v>
       </c>
@@ -2911,11 +3626,22 @@
         <v>31.754000000000001</v>
       </c>
       <c r="F87">
-        <f>D87-E87</f>
+        <f t="shared" si="6"/>
         <v>36.440999999999988</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <v>37.811999999999998</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="7"/>
+        <v>2.8912250079339885</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="8"/>
+        <v>1.8035279805352797</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>67</v>
       </c>
@@ -2932,11 +3658,22 @@
         <v>27.06</v>
       </c>
       <c r="F88">
-        <f>D88-E88</f>
+        <f t="shared" si="6"/>
         <v>14.440999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <v>23.076000000000001</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="7"/>
+        <v>1.877405096203848</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="8"/>
+        <v>1.798448604610851</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>68</v>
       </c>
@@ -2953,11 +3690,22 @@
         <v>25.388999999999999</v>
       </c>
       <c r="F89">
-        <f>D89-E89</f>
+        <f t="shared" si="6"/>
         <v>20.564000000000004</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <v>23.995999999999999</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="7"/>
+        <v>2.5709284880813477</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="8"/>
+        <v>1.9150275045840977</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -2974,11 +3722,22 @@
         <v>36.387</v>
       </c>
       <c r="F90">
-        <f>D90-E90</f>
+        <f t="shared" si="6"/>
         <v>14.772999999999996</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <v>27.378</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="7"/>
+        <v>1.6187815033968875</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="8"/>
+        <v>1.8686536635254583</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>70</v>
       </c>
@@ -2995,11 +3754,22 @@
         <v>16.623000000000001</v>
       </c>
       <c r="F91">
-        <f>D91-E91</f>
+        <f t="shared" si="6"/>
         <v>7.3739999999999988</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <v>19.725999999999999</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="7"/>
+        <v>1.1214640575889687</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="8"/>
+        <v>1.216516272939268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -3016,11 +3786,22 @@
         <v>24.355</v>
       </c>
       <c r="F92">
-        <f>D92-E92</f>
+        <f t="shared" si="6"/>
         <v>14.754000000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <v>25.102</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="7"/>
+        <v>1.7632857939606408</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="8"/>
+        <v>1.5580033463469047</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>72</v>
       </c>
@@ -3037,11 +3818,22 @@
         <v>20.099</v>
       </c>
       <c r="F93">
-        <f>D93-E93</f>
+        <f t="shared" si="6"/>
         <v>16.232000000000003</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <v>21.018000000000001</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="7"/>
+        <v>2.3168712532115334</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="8"/>
+        <v>1.728565991055286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>73</v>
       </c>
@@ -3058,11 +3850,22 @@
         <v>32.738999999999997</v>
       </c>
       <c r="F94">
-        <f>D94-E94</f>
+        <f t="shared" si="6"/>
         <v>13.61</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <v>34.488</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="7"/>
+        <v>1.1838900487125956</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="8"/>
+        <v>1.3439167246578518</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>74</v>
       </c>
@@ -3079,11 +3882,22 @@
         <v>28.18</v>
       </c>
       <c r="F95">
-        <f>D95-E95</f>
+        <f t="shared" si="6"/>
         <v>14.692</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <v>22.486000000000001</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="7"/>
+        <v>1.9601529840789826</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="8"/>
+        <v>1.9066085564351152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>75</v>
       </c>
@@ -3100,11 +3914,22 @@
         <v>21.138999999999999</v>
       </c>
       <c r="F96">
-        <f>D96-E96</f>
+        <f t="shared" si="6"/>
         <v>11.291</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <v>17.135999999999999</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="7"/>
+        <v>1.9767156862745101</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="8"/>
+        <v>1.8925070028011206</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>76</v>
       </c>
@@ -3121,11 +3946,22 @@
         <v>30.126000000000001</v>
       </c>
       <c r="F97">
-        <f>D97-E97</f>
+        <f t="shared" si="6"/>
         <v>19.989999999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <v>33.036000000000001</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="7"/>
+        <v>1.815292408281874</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="8"/>
+        <v>1.5170117447632885</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>77</v>
       </c>
@@ -3142,11 +3978,22 @@
         <v>28.082000000000001</v>
       </c>
       <c r="F98">
-        <f>D98-E98</f>
+        <f t="shared" ref="F98:F140" si="9">D98-E98</f>
         <v>12.402999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <v>18.155999999999999</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="7"/>
+        <v>2.0494051553205552</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="8"/>
+        <v>2.2298413747521484</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>78</v>
       </c>
@@ -3163,11 +4010,22 @@
         <v>19.744</v>
       </c>
       <c r="F99">
-        <f>D99-E99</f>
+        <f t="shared" si="9"/>
         <v>9.4510000000000005</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <v>17.931999999999999</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="7"/>
+        <v>1.5811398616997547</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="8"/>
+        <v>1.6280950256524651</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>79</v>
       </c>
@@ -3184,11 +4042,22 @@
         <v>28.026</v>
       </c>
       <c r="F100">
-        <f>D100-E100</f>
+        <f t="shared" si="9"/>
         <v>9.9139999999999979</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <v>23.681999999999999</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="7"/>
+        <v>1.2558905497846462</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="8"/>
+        <v>1.602060636770543</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>80</v>
       </c>
@@ -3205,11 +4074,22 @@
         <v>27.975000000000001</v>
       </c>
       <c r="F101">
-        <f>D101-E101</f>
+        <f t="shared" si="9"/>
         <v>19.198</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <v>20.001999999999999</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="7"/>
+        <v>2.879412058794121</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="8"/>
+        <v>2.3584141585841416</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>81</v>
       </c>
@@ -3226,11 +4106,22 @@
         <v>25.619</v>
       </c>
       <c r="F102">
-        <f>D102-E102</f>
+        <f t="shared" si="9"/>
         <v>10.439999999999998</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <v>23.053999999999998</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="7"/>
+        <v>1.358549492495879</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="8"/>
+        <v>1.5641103496139499</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>82</v>
       </c>
@@ -3247,11 +4138,22 @@
         <v>23.558</v>
       </c>
       <c r="F103">
-        <f>D103-E103</f>
+        <f t="shared" si="9"/>
         <v>16.103999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <v>20.698</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="7"/>
+        <v>2.3341385641124743</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="8"/>
+        <v>1.9162237897381389</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>83</v>
       </c>
@@ -3268,11 +4170,22 @@
         <v>28.132999999999999</v>
       </c>
       <c r="F104">
-        <f>D104-E104</f>
+        <f t="shared" si="9"/>
         <v>34.742000000000004</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <v>29.24</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="7"/>
+        <v>3.5645006839945288</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="8"/>
+        <v>2.1503077975376197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>84</v>
       </c>
@@ -3289,11 +4202,22 @@
         <v>25.417999999999999</v>
       </c>
       <c r="F105">
-        <f>D105-E105</f>
+        <f t="shared" si="9"/>
         <v>18.228999999999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <v>23.99</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="7"/>
+        <v>2.2795748228428514</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="8"/>
+        <v>1.8193830762817842</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>85</v>
       </c>
@@ -3310,11 +4234,22 @@
         <v>24.225999999999999</v>
       </c>
       <c r="F106">
-        <f>D106-E106</f>
+        <f t="shared" si="9"/>
         <v>19.5</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <v>27.97</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="7"/>
+        <v>2.0915266356810869</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="8"/>
+        <v>1.5633178405434394</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>86</v>
       </c>
@@ -3331,11 +4266,22 @@
         <v>22.722999999999999</v>
       </c>
       <c r="F107">
-        <f>D107-E107</f>
+        <f t="shared" si="9"/>
         <v>14.803000000000004</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <v>22.062000000000001</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="7"/>
+        <v>2.012918139787871</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="8"/>
+        <v>1.7009337322092286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>87</v>
       </c>
@@ -3352,11 +4298,22 @@
         <v>29.574999999999999</v>
       </c>
       <c r="F108">
-        <f>D108-E108</f>
+        <f t="shared" si="9"/>
         <v>13.714000000000002</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <v>29.83</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="7"/>
+        <v>1.3792155548105938</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="8"/>
+        <v>1.4511900771035871</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>88</v>
       </c>
@@ -3373,11 +4330,22 @@
         <v>33.793999999999997</v>
       </c>
       <c r="F109">
-        <f>D109-E109</f>
+        <f t="shared" si="9"/>
         <v>32.781999999999996</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <v>41.305</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="7"/>
+        <v>2.3809708267764189</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="8"/>
+        <v>1.6118145502965742</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>89</v>
       </c>
@@ -3394,11 +4362,22 @@
         <v>28.884</v>
       </c>
       <c r="F110">
-        <f>D110-E110</f>
+        <f t="shared" si="9"/>
         <v>27.746000000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <v>34.192</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="7"/>
+        <v>2.4344291062236785</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="8"/>
+        <v>1.6562353766963034</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>90</v>
       </c>
@@ -3415,11 +4394,22 @@
         <v>26.802</v>
       </c>
       <c r="F111">
-        <f>D111-E111</f>
+        <f t="shared" si="9"/>
         <v>13.244</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <v>25.396000000000001</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="7"/>
+        <v>1.5644983461962512</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="8"/>
+        <v>1.5768624980311858</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>91</v>
       </c>
@@ -3436,11 +4426,22 @@
         <v>32.628</v>
       </c>
       <c r="F112">
-        <f>D112-E112</f>
+        <f t="shared" si="9"/>
         <v>41.168000000000006</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <v>37.052</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="7"/>
+        <v>3.333261362409587</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="8"/>
+        <v>1.9916873583072441</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>92</v>
       </c>
@@ -3457,11 +4458,22 @@
         <v>29.323</v>
       </c>
       <c r="F113">
-        <f>D113-E113</f>
+        <f t="shared" si="9"/>
         <v>34.937999999999995</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G113">
+        <v>29.67</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="7"/>
+        <v>3.5326592517694637</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="8"/>
+        <v>2.1658577687900231</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>93</v>
       </c>
@@ -3478,11 +4490,22 @@
         <v>25.559000000000001</v>
       </c>
       <c r="F114">
-        <f>D114-E114</f>
+        <f t="shared" si="9"/>
         <v>9.1709999999999958</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G114">
+        <v>22.084</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="7"/>
+        <v>1.2458340880275307</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="8"/>
+        <v>1.5726317696069552</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>94</v>
       </c>
@@ -3499,11 +4522,22 @@
         <v>24.719000000000001</v>
       </c>
       <c r="F115">
-        <f>D115-E115</f>
+        <f t="shared" si="9"/>
         <v>13.746000000000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G115">
+        <v>21.745999999999999</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="7"/>
+        <v>1.8963487537938017</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="8"/>
+        <v>1.7688310493883936</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>95</v>
       </c>
@@ -3520,11 +4554,22 @@
         <v>19.048999999999999</v>
       </c>
       <c r="F116">
-        <f>D116-E116</f>
+        <f t="shared" si="9"/>
         <v>11.964000000000002</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G116">
+        <v>16.565999999999999</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="7"/>
+        <v>2.1666063020644697</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="8"/>
+        <v>1.8720874079439818</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>96</v>
       </c>
@@ -3541,11 +4586,22 @@
         <v>21.553000000000001</v>
       </c>
       <c r="F117">
-        <f>D117-E117</f>
+        <f t="shared" si="9"/>
         <v>15.126999999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G117">
+        <v>18.091999999999999</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="7"/>
+        <v>2.5083462303780677</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="8"/>
+        <v>2.0274154322352422</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>97</v>
       </c>
@@ -3562,11 +4618,22 @@
         <v>28.326000000000001</v>
       </c>
       <c r="F118">
-        <f>D118-E118</f>
+        <f t="shared" si="9"/>
         <v>11.494999999999997</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G118">
+        <v>23.431999999999999</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="7"/>
+        <v>1.4717053601911914</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="8"/>
+        <v>1.6994281324684193</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>98</v>
       </c>
@@ -3583,11 +4650,22 @@
         <v>22.47</v>
       </c>
       <c r="F119">
-        <f>D119-E119</f>
+        <f t="shared" si="9"/>
         <v>13.953000000000003</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G119">
+        <v>16.119</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="7"/>
+        <v>2.5968732551647129</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="8"/>
+        <v>2.2596314907872697</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>99</v>
       </c>
@@ -3604,11 +4682,22 @@
         <v>29.536000000000001</v>
       </c>
       <c r="F120">
-        <f>D120-E120</f>
+        <f t="shared" si="9"/>
         <v>20.795999999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G120">
+        <v>26.021999999999998</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="7"/>
+        <v>2.3975097994005075</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="8"/>
+        <v>1.9342095150257477</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>100</v>
       </c>
@@ -3625,11 +4714,22 @@
         <v>28.39</v>
       </c>
       <c r="F121">
-        <f>D121-E121</f>
+        <f t="shared" si="9"/>
         <v>23.622</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G121">
+        <v>27.545999999999999</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="7"/>
+        <v>2.5726421258984971</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="8"/>
+        <v>1.8881870326000145</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>101</v>
       </c>
@@ -3646,11 +4746,22 @@
         <v>33.353999999999999</v>
       </c>
       <c r="F122">
-        <f>D122-E122</f>
+        <f t="shared" si="9"/>
         <v>45.796000000000006</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G122">
+        <v>35.869999999999997</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="7"/>
+        <v>3.8301644828547543</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="8"/>
+        <v>2.2065793141901313</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>102</v>
       </c>
@@ -3667,11 +4778,22 @@
         <v>25.263000000000002</v>
       </c>
       <c r="F123">
-        <f>D123-E123</f>
+        <f t="shared" si="9"/>
         <v>12.883999999999997</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G123">
+        <v>20.09</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="7"/>
+        <v>1.9239422598307612</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="8"/>
+        <v>1.8988053758088601</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>103</v>
       </c>
@@ -3688,11 +4810,22 @@
         <v>27.885999999999999</v>
       </c>
       <c r="F124">
-        <f>D124-E124</f>
+        <f t="shared" si="9"/>
         <v>20.428999999999998</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G124">
+        <v>23.608000000000001</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="7"/>
+        <v>2.5960267705862416</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="8"/>
+        <v>2.0465520162656725</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>104</v>
       </c>
@@ -3709,83 +4842,499 @@
         <v>25.571000000000002</v>
       </c>
       <c r="F125">
-        <f>D125-E125</f>
+        <f t="shared" si="9"/>
         <v>18.605</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G125">
+        <v>21.192</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="7"/>
+        <v>2.6337768969422424</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="8"/>
+        <v>2.0845602114005284</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>101</v>
+      </c>
+      <c r="C126" t="s">
+        <v>108</v>
+      </c>
+      <c r="D126">
+        <v>38.564999999999998</v>
+      </c>
+      <c r="E126">
+        <v>21.457000000000001</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="9"/>
+        <v>17.107999999999997</v>
+      </c>
+      <c r="G126">
+        <v>19.763999999999999</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="7"/>
+        <v>2.5968427443837276</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="8"/>
+        <v>1.9512750455373407</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>25</v>
+      </c>
+      <c r="C127" t="s">
+        <v>105</v>
+      </c>
+      <c r="D127">
+        <v>39.853000000000002</v>
+      </c>
+      <c r="E127">
+        <v>28.016999999999999</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="9"/>
+        <v>11.836000000000002</v>
+      </c>
+      <c r="G127">
+        <v>16.756</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="7"/>
+        <v>2.1191215087132971</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="8"/>
+        <v>2.3784316065886846</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>93</v>
+      </c>
+      <c r="C128" t="s">
+        <v>108</v>
+      </c>
+      <c r="D128">
+        <v>16.23</v>
+      </c>
+      <c r="E128">
+        <v>11.275</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="9"/>
+        <v>4.9550000000000001</v>
+      </c>
+      <c r="G128">
+        <v>16.077000000000002</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="7"/>
+        <v>0.92461280089568931</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="8"/>
+        <v>1.0095167008770292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>152</v>
+      </c>
+      <c r="C129" t="s">
+        <v>109</v>
+      </c>
+      <c r="D129">
+        <v>33.154000000000003</v>
+      </c>
+      <c r="E129">
+        <v>20.506</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="9"/>
+        <v>12.648000000000003</v>
+      </c>
+      <c r="G129">
+        <v>22.364000000000001</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="7"/>
+        <v>1.6966553389375787</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="8"/>
+        <v>1.4824718297263459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>38</v>
+      </c>
+      <c r="C130" t="s">
+        <v>105</v>
+      </c>
+      <c r="D130">
+        <v>49.753</v>
+      </c>
+      <c r="E130">
+        <v>32.673999999999999</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="9"/>
+        <v>17.079000000000001</v>
+      </c>
+      <c r="G130">
+        <v>25.864000000000001</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="7"/>
+        <v>1.9810160841323849</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="8"/>
+        <v>1.9236390349520569</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>120</v>
+      </c>
+      <c r="C131" t="s">
+        <v>108</v>
+      </c>
+      <c r="D131">
+        <v>31.006</v>
+      </c>
+      <c r="E131">
+        <v>18.792999999999999</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="9"/>
+        <v>12.213000000000001</v>
+      </c>
+      <c r="G131">
+        <v>18.128</v>
+      </c>
+      <c r="H131">
+        <f t="shared" si="7"/>
+        <v>2.0211275375110329</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="8"/>
+        <v>1.7103927625772286</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>87</v>
+      </c>
+      <c r="C132" t="s">
+        <v>108</v>
+      </c>
+      <c r="D132">
+        <v>39.07</v>
+      </c>
+      <c r="E132">
+        <v>22.347999999999999</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="9"/>
+        <v>16.722000000000001</v>
+      </c>
+      <c r="G132">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="H132">
+        <f t="shared" si="7"/>
+        <v>2.5272544080604535</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="8"/>
+        <v>1.9682619647355162</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>168</v>
+      </c>
+      <c r="C133" t="s">
+        <v>109</v>
+      </c>
+      <c r="D133">
+        <v>21.625</v>
+      </c>
+      <c r="E133">
+        <v>14.611000000000001</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="9"/>
+        <v>7.0139999999999993</v>
+      </c>
+      <c r="G133">
+        <v>12.545</v>
+      </c>
+      <c r="H133">
+        <f t="shared" si="7"/>
+        <v>1.6773216420884816</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="8"/>
+        <v>1.7237943403746512</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>35</v>
+      </c>
+      <c r="C134" t="s">
+        <v>105</v>
+      </c>
+      <c r="D134">
+        <v>47.451000000000001</v>
+      </c>
+      <c r="E134">
+        <v>30.835000000000001</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="9"/>
+        <v>16.616</v>
+      </c>
+      <c r="G134">
+        <v>22.332000000000001</v>
+      </c>
+      <c r="H134">
+        <f t="shared" si="7"/>
+        <v>2.2321332616872649</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="8"/>
+        <v>2.1247984954325632</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>41</v>
+      </c>
+      <c r="C135" t="s">
+        <v>105</v>
+      </c>
+      <c r="D135">
+        <v>35.960999999999999</v>
+      </c>
+      <c r="E135">
+        <v>24.289000000000001</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="9"/>
+        <v>11.671999999999997</v>
+      </c>
+      <c r="G135">
+        <v>17.442</v>
+      </c>
+      <c r="H135">
+        <f t="shared" si="7"/>
+        <v>2.0075679394564836</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="8"/>
+        <v>2.0617475060199517</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>19</v>
+      </c>
+      <c r="C136" t="s">
+        <v>105</v>
+      </c>
+      <c r="D136">
+        <v>43.317</v>
+      </c>
+      <c r="E136">
+        <v>30.120999999999999</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="9"/>
+        <v>13.196000000000002</v>
+      </c>
+      <c r="G136">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="7"/>
+        <v>1.5901349614395888</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="8"/>
+        <v>1.739918059125964</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>92</v>
+      </c>
+      <c r="C137" t="s">
+        <v>108</v>
+      </c>
+      <c r="D137">
+        <v>29.876000000000001</v>
+      </c>
+      <c r="E137">
+        <v>18.288</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="9"/>
+        <v>11.588000000000001</v>
+      </c>
+      <c r="G137">
+        <v>23.152000000000001</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="7"/>
+        <v>1.5015549412577749</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="8"/>
+        <v>1.2904284727021424</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>82</v>
+      </c>
+      <c r="C138" t="s">
+        <v>107</v>
+      </c>
+      <c r="D138">
+        <v>41.896999999999998</v>
+      </c>
+      <c r="E138">
+        <v>28.382000000000001</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="9"/>
+        <v>13.514999999999997</v>
+      </c>
+      <c r="G138">
+        <v>20.024000000000001</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="7"/>
+        <v>2.0248202157411104</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="8"/>
+        <v>2.0923391929684376</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>81</v>
+      </c>
+      <c r="C139" t="s">
+        <v>107</v>
+      </c>
+      <c r="D139">
+        <v>47.832000000000001</v>
+      </c>
+      <c r="E139">
+        <v>34.515000000000001</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="9"/>
+        <v>13.317</v>
+      </c>
+      <c r="G139">
+        <v>26.655999999999999</v>
+      </c>
+      <c r="H139">
+        <f t="shared" si="7"/>
+        <v>1.4987620048019208</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="8"/>
+        <v>1.7944177671068429</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>150</v>
+      </c>
+      <c r="B140">
+        <v>47</v>
+      </c>
+      <c r="C140" t="s">
+        <v>107</v>
+      </c>
+      <c r="D140">
+        <v>26.364999999999998</v>
+      </c>
+      <c r="E140">
+        <v>16.849</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="9"/>
+        <v>9.5159999999999982</v>
+      </c>
+      <c r="G140">
+        <v>18.391999999999999</v>
+      </c>
+      <c r="H140">
+        <f t="shared" si="7"/>
+        <v>1.5521966072205307</v>
+      </c>
+      <c r="I140">
+        <f t="shared" si="8"/>
+        <v>1.433503697259678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>